<commit_message>
Implemented Status tracking column in TransactionData to conform to solution standards
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\uipath-automation-4\ProjectPlagiarismBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515F1993-244C-4F11-893C-AE08EA37D396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E47DC7-B814-4E36-AE84-4E6EC6A29DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20870" yWindow="610" windowWidth="17280" windowHeight="8980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -140,6 +140,33 @@
   </si>
   <si>
     <t>C:\Users\angel\GitHub\uipath-automation-4\ProjectPlagiarismBot\Data\Output</t>
+  </si>
+  <si>
+    <t>Status_Success</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record successful transaction.</t>
+  </si>
+  <si>
+    <t>Status_Failure</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record failed transaction.</t>
+  </si>
+  <si>
+    <t>Status_Pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record pending transaction.</t>
   </si>
 </sst>
 </file>
@@ -517,14 +544,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -573,7 +600,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="29">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1609,14 +1636,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1653,7 +1682,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1733,9 +1762,39 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2723,12 +2782,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
added annotations and tested adding some things
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-4\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Training/ProjectPlagiarismBot/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E47DC7-B814-4E36-AE84-4E6EC6A29DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{35E47DC7-B814-4E36-AE84-4E6EC6A29DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC48030B-9F71-434E-93A1-2AC1A170B0C4}"/>
   <bookViews>
-    <workbookView xWindow="20870" yWindow="610" windowWidth="17280" windowHeight="8980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="19200" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>C:\Users\angel\GitHub\uipath-automation-4\ProjectPlagiarismBot\Data\Input\GitHubRepoURLInput.CSV</t>
-  </si>
-  <si>
     <t>InputCSVFilePath</t>
   </si>
   <si>
@@ -136,12 +133,6 @@
     <t>GitCloneRootFilePath</t>
   </si>
   <si>
-    <t>C:\Users\angel\GitHub\uipath-automation-4\ProjectPlagiarismBot\GitRepoCloning</t>
-  </si>
-  <si>
-    <t>C:\Users\angel\GitHub\uipath-automation-4\ProjectPlagiarismBot\Data\Output</t>
-  </si>
-  <si>
     <t>Status_Success</t>
   </si>
   <si>
@@ -167,6 +158,15 @@
   </si>
   <si>
     <t>Status message for TransactionData to record pending transaction.</t>
+  </si>
+  <si>
+    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Input\GitHubRepoURLInput.CSV</t>
+  </si>
+  <si>
+    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Input\GitRepoCloning</t>
+  </si>
+  <si>
+    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Output</t>
   </si>
 </sst>
 </file>
@@ -544,14 +544,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -600,7 +602,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="29">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -614,26 +616,26 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1636,16 +1638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1682,7 +1684,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1764,35 +1766,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2782,12 +2784,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.1796875" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
working branch conforming to best practices branch in forked repo
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Training/ProjectPlagiarismBot/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{35E47DC7-B814-4E36-AE84-4E6EC6A29DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC48030B-9F71-434E-93A1-2AC1A170B0C4}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{35E47DC7-B814-4E36-AE84-4E6EC6A29DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C67153FD-C9F1-4D68-AC2D-5055FE70A1D0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="19200" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="630" windowWidth="10200" windowHeight="9470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -127,12 +127,6 @@
     <t>InputCSVFilePath</t>
   </si>
   <si>
-    <t>GitDiffOutputFilePath</t>
-  </si>
-  <si>
-    <t>GitCloneRootFilePath</t>
-  </si>
-  <si>
     <t>Status_Success</t>
   </si>
   <si>
@@ -160,13 +154,37 @@
     <t>Status message for TransactionData to record pending transaction.</t>
   </si>
   <si>
-    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Input\GitHubRepoURLInput.CSV</t>
-  </si>
-  <si>
-    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Input\GitRepoCloning</t>
-  </si>
-  <si>
-    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Output</t>
+    <t>Data\Input\GitHubRepoURLInput.csv</t>
+  </si>
+  <si>
+    <t>A relative path pointing to a place to look for the input CSV file before asking the user for input.</t>
+  </si>
+  <si>
+    <t>GitCloneRepoATargetPath</t>
+  </si>
+  <si>
+    <t>Data\Temp\RepoA</t>
+  </si>
+  <si>
+    <t>A relative path pointing to a place to clone the first repo in each transaction to be compared.</t>
+  </si>
+  <si>
+    <t>GitCloneRepoBTargetPath</t>
+  </si>
+  <si>
+    <t>Data\Temp\RepoB</t>
+  </si>
+  <si>
+    <t>A relative path pointing to a place to clone thesecond repo in each transaction to be compared.</t>
+  </si>
+  <si>
+    <t>GitDiffOutputFolderPath</t>
+  </si>
+  <si>
+    <t>A relative path pointing to a place to store the diff outputs for the repositories to be compared.</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -218,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -228,6 +246,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -615,30 +634,49 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1766,35 +1804,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated Config with Azure Authentication; Added ReadMe
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\uipath-automation-4\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e005f2666f30fec7/Documents/UiPath/uipath-automation-4/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C1B49F-5784-4ACD-8837-B5D7C9437FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E2C1B49F-5784-4ACD-8837-B5D7C9437FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9803452D-7F95-4DF1-A0C4-42E31E86A18D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9756" yWindow="2244" windowWidth="19344" windowHeight="12768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -185,13 +185,28 @@
   </si>
   <si>
     <t>Folder path to save Output Matrix</t>
+  </si>
+  <si>
+    <t>Azure_Tenant_Id</t>
+  </si>
+  <si>
+    <t>7a2c76a6-7919-4b03-86fd-888499c49d2b</t>
+  </si>
+  <si>
+    <t>Azure_App_Id</t>
+  </si>
+  <si>
+    <t>b8330c48-358c-4528-84a4-ec385e3aa70b</t>
+  </si>
+  <si>
+    <t>Needed for Microsoft Office 365 Activities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -215,6 +230,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -247,6 +268,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,16 +585,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -621,7 +643,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="29">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1674,16 +1696,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1720,7 +1742,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1834,23 +1856,43 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2809,6 +2851,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2820,12 +2863,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>